<commit_message>
generate intended recipient extension 6c6622d5fa114ffaeb873ed27aebfa06bf70d2e0
</commit_message>
<xml_diff>
--- a/ig/nr-update-deps/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr-update-deps/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-07T14:11:56+00:00</t>
+    <t>2024-02-07T14:52:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -647,7 +647,7 @@
     <t>isArchived</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/pdsm-is-archived}
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/pdsm/StructureDefinition/pdsm-ext-is-archived}
 </t>
   </si>
   <si>

</xml_diff>